<commit_message>
cosmetic amendment on test case backlog
</commit_message>
<xml_diff>
--- a/2.Automation_backlog.xlsx
+++ b/2.Automation_backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="725" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" tabRatio="725"/>
   </bookViews>
   <sheets>
     <sheet name="Test cases" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,13 @@
     <sheet name="Account management tests" sheetId="12" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Account management tests'!$A$1:$G$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Account management tests'!$A$1:$G$86</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Checkout test'!$A$1:$G$68</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Compare product tests'!$A$1:$G$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Forgotten Password'!$A$1:$G$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Login Tests'!$A$1:$G$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Regsitration Tests'!$A$1:$G$140</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Search tests'!$A$1:$G$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Search tests'!$A$1:$G$130</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Shopping cart tests'!$A$1:$G$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Wishlist tests'!$A$1:$G$9</definedName>
   </definedNames>
@@ -1498,7 +1500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1697,9 +1699,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2044,8 +2043,8 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2098,7 +2097,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="15">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.35">
@@ -2128,8 +2127,8 @@
       <c r="C5" s="2">
         <v>28</v>
       </c>
-      <c r="D5" s="94">
-        <v>3</v>
+      <c r="D5" s="15">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -2142,8 +2141,8 @@
       <c r="C6" s="93">
         <v>10</v>
       </c>
-      <c r="D6" s="93">
-        <v>1</v>
+      <c r="D6" s="15">
+        <v>2</v>
       </c>
       <c r="E6"/>
       <c r="F6"/>
@@ -2159,7 +2158,7 @@
       <c r="C7" s="93">
         <v>4</v>
       </c>
-      <c r="D7" s="93">
+      <c r="D7" s="15">
         <v>0</v>
       </c>
     </row>
@@ -2173,7 +2172,7 @@
       <c r="C8" s="93">
         <v>4</v>
       </c>
-      <c r="D8" s="93">
+      <c r="D8" s="15">
         <v>0</v>
       </c>
     </row>
@@ -2187,8 +2186,8 @@
       <c r="C9" s="93">
         <v>11</v>
       </c>
-      <c r="D9">
-        <v>3</v>
+      <c r="D9" s="15">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2214,7 +2213,7 @@
       </c>
       <c r="D11" s="7">
         <f>SUM(D2:D10)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2227,9 +2226,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E143" sqref="E143"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2279,11 +2278,11 @@
       <c r="D2" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="E2" s="96" t="s">
+      <c r="E2" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="F2" s="97"/>
-      <c r="G2" s="98" t="s">
+      <c r="F2" s="96"/>
+      <c r="G2" s="97" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2427,11 +2426,11 @@
       <c r="D14" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="E14" s="96" t="s">
+      <c r="E14" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="F14" s="97"/>
-      <c r="G14" s="98" t="s">
+      <c r="F14" s="96"/>
+      <c r="G14" s="97" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2641,11 +2640,11 @@
       <c r="D32" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="E32" s="96" t="s">
+      <c r="E32" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="F32" s="97"/>
-      <c r="G32" s="98" t="s">
+      <c r="F32" s="96"/>
+      <c r="G32" s="97" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3534,7 +3533,7 @@
         <v>112</v>
       </c>
       <c r="F107" s="74"/>
-      <c r="G107" s="102" t="s">
+      <c r="G107" s="101" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3916,9 +3915,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E79" sqref="E79"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3968,11 +3967,11 @@
       <c r="D2" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="E2" s="96" t="s">
+      <c r="E2" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="F2" s="97"/>
-      <c r="G2" s="98" t="s">
+      <c r="F2" s="96"/>
+      <c r="G2" s="97" t="s">
         <v>25</v>
       </c>
     </row>
@@ -4072,7 +4071,7 @@
       <c r="D10" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="E10" s="96" t="s">
+      <c r="E10" s="95" t="s">
         <v>112</v>
       </c>
       <c r="F10" s="25"/>
@@ -4154,7 +4153,7 @@
       <c r="D16" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="E16" s="96" t="s">
+      <c r="E16" s="95" t="s">
         <v>112</v>
       </c>
       <c r="F16" s="25"/>
@@ -4313,7 +4312,7 @@
       <c r="D29" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="E29" s="96" t="s">
+      <c r="E29" s="95" t="s">
         <v>112</v>
       </c>
       <c r="F29" s="25"/>
@@ -4373,7 +4372,7 @@
       <c r="D33" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="E33" s="96" t="s">
+      <c r="E33" s="95" t="s">
         <v>112</v>
       </c>
       <c r="F33" s="25"/>
@@ -4402,10 +4401,10 @@
       <c r="B36" s="51"/>
       <c r="C36" s="51"/>
       <c r="D36" s="51"/>
-      <c r="E36" s="99" t="s">
+      <c r="E36" s="98" t="s">
         <v>273</v>
       </c>
-      <c r="F36" s="100" t="s">
+      <c r="F36" s="99" t="s">
         <v>274</v>
       </c>
       <c r="G36" s="76"/>
@@ -4423,7 +4422,7 @@
       <c r="D37" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="E37" s="96" t="s">
+      <c r="E37" s="95" t="s">
         <v>112</v>
       </c>
       <c r="F37" s="25"/>
@@ -4456,10 +4455,10 @@
       <c r="B40" s="51"/>
       <c r="C40" s="51"/>
       <c r="D40" s="51"/>
-      <c r="E40" s="99" t="s">
+      <c r="E40" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="F40" s="100" t="s">
+      <c r="F40" s="99" t="s">
         <v>254</v>
       </c>
       <c r="G40" s="76"/>
@@ -4477,7 +4476,7 @@
       <c r="D41" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="E41" s="96" t="s">
+      <c r="E41" s="95" t="s">
         <v>112</v>
       </c>
       <c r="F41" s="25"/>
@@ -4517,10 +4516,10 @@
       <c r="B45" s="51"/>
       <c r="C45" s="51"/>
       <c r="D45" s="51"/>
-      <c r="E45" s="99" t="s">
+      <c r="E45" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="F45" s="100" t="s">
+      <c r="F45" s="99" t="s">
         <v>254</v>
       </c>
       <c r="G45" s="76"/>
@@ -4538,7 +4537,7 @@
       <c r="D46" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="E46" s="96" t="s">
+      <c r="E46" s="95" t="s">
         <v>112</v>
       </c>
       <c r="F46" s="25"/>
@@ -4586,10 +4585,10 @@
       <c r="B50" s="51"/>
       <c r="C50" s="51"/>
       <c r="D50" s="51"/>
-      <c r="E50" s="99" t="s">
+      <c r="E50" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="F50" s="100" t="s">
+      <c r="F50" s="99" t="s">
         <v>254</v>
       </c>
       <c r="G50" s="76"/>
@@ -4607,7 +4606,7 @@
       <c r="D51" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="E51" s="96" t="s">
+      <c r="E51" s="95" t="s">
         <v>112</v>
       </c>
       <c r="F51" s="25"/>
@@ -4703,10 +4702,10 @@
       <c r="B60" s="51"/>
       <c r="C60" s="51"/>
       <c r="D60" s="51"/>
-      <c r="E60" s="99" t="s">
+      <c r="E60" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="F60" s="100" t="s">
+      <c r="F60" s="99" t="s">
         <v>254</v>
       </c>
       <c r="G60" s="76"/>
@@ -4724,7 +4723,7 @@
       <c r="D61" s="25" t="s">
         <v>363</v>
       </c>
-      <c r="E61" s="103" t="s">
+      <c r="E61" s="102" t="s">
         <v>112</v>
       </c>
       <c r="F61" s="24"/>
@@ -4759,13 +4758,13 @@
       <c r="B64" s="77"/>
       <c r="C64" s="77"/>
       <c r="D64" s="77"/>
-      <c r="E64" s="104" t="s">
+      <c r="E64" s="103" t="s">
         <v>364</v>
       </c>
       <c r="F64" s="77" t="s">
         <v>365</v>
       </c>
-      <c r="G64" s="95"/>
+      <c r="G64" s="94"/>
     </row>
     <row r="65" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
@@ -4780,7 +4779,7 @@
       <c r="D65" s="25" t="s">
         <v>363</v>
       </c>
-      <c r="E65" s="103" t="s">
+      <c r="E65" s="102" t="s">
         <v>112</v>
       </c>
       <c r="F65" s="24"/>
@@ -4813,7 +4812,7 @@
       <c r="B68" s="31"/>
       <c r="C68" s="31"/>
       <c r="D68" s="31"/>
-      <c r="E68" s="105" t="s">
+      <c r="E68" s="104" t="s">
         <v>364</v>
       </c>
       <c r="F68" s="31"/>
@@ -4824,7 +4823,7 @@
       <c r="B69" s="51"/>
       <c r="C69" s="51"/>
       <c r="D69" s="51"/>
-      <c r="E69" s="104" t="s">
+      <c r="E69" s="103" t="s">
         <v>367</v>
       </c>
       <c r="F69" s="51" t="s">
@@ -4845,7 +4844,7 @@
       <c r="D70" s="25" t="s">
         <v>363</v>
       </c>
-      <c r="E70" s="103" t="s">
+      <c r="E70" s="102" t="s">
         <v>112</v>
       </c>
       <c r="F70" s="24"/>
@@ -4880,7 +4879,7 @@
       <c r="B73" s="31"/>
       <c r="C73" s="31"/>
       <c r="D73" s="31"/>
-      <c r="E73" s="105" t="s">
+      <c r="E73" s="104" t="s">
         <v>364</v>
       </c>
       <c r="F73" s="31"/>
@@ -4888,7 +4887,7 @@
     </row>
     <row r="74" spans="1:7" s="31" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="24"/>
-      <c r="E74" s="105" t="s">
+      <c r="E74" s="104" t="s">
         <v>369</v>
       </c>
       <c r="G74" s="75"/>
@@ -4948,7 +4947,7 @@
       <c r="D79" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="E79" s="103" t="s">
+      <c r="E79" s="102" t="s">
         <v>112</v>
       </c>
       <c r="F79" s="24"/>
@@ -5023,7 +5022,7 @@
       <c r="B86" s="51"/>
       <c r="C86" s="51"/>
       <c r="D86" s="51"/>
-      <c r="E86" s="101" t="s">
+      <c r="E86" s="100" t="s">
         <v>22</v>
       </c>
       <c r="F86" s="51" t="s">
@@ -5032,7 +5031,7 @@
       <c r="G86" s="76"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G32"/>
+  <autoFilter ref="A1:G86"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5718,11 +5717,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12:G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5758,7 +5758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="14"/>
       <c r="C3" s="15"/>
@@ -5792,7 +5792,7 @@
       </c>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13"/>
       <c r="B4" s="14"/>
       <c r="C4" s="15"/>
@@ -5803,7 +5803,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
       <c r="B5" s="14"/>
       <c r="C5" s="15"/>
@@ -5814,7 +5814,7 @@
       <c r="F5" s="14"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13"/>
       <c r="B6" s="14"/>
       <c r="C6" s="15"/>
@@ -5825,7 +5825,7 @@
       <c r="F6" s="14"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13"/>
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
@@ -5836,7 +5836,7 @@
       <c r="F7" s="14"/>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13"/>
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
@@ -5847,7 +5847,7 @@
       <c r="F8" s="14"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -5858,7 +5858,7 @@
       <c r="F9" s="14"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
@@ -5869,7 +5869,7 @@
       <c r="F10" s="14"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
@@ -5903,7 +5903,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B13" s="14"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -5915,7 +5915,7 @@
       </c>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -5925,7 +5925,7 @@
       <c r="F14" s="14"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -5935,7 +5935,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="16"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B16" s="14"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -5945,7 +5945,7 @@
       <c r="F16" s="14"/>
       <c r="G16" s="16"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -5955,7 +5955,7 @@
       <c r="F17" s="14"/>
       <c r="G17" s="16"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
@@ -5965,7 +5965,7 @@
       <c r="F18" s="14"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -5975,7 +5975,7 @@
       <c r="F19" s="14"/>
       <c r="G19" s="16"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B20" s="14"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -5985,7 +5985,7 @@
       <c r="F20" s="14"/>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="51"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19"/>
@@ -5998,7 +5998,7 @@
       </c>
       <c r="G21" s="20"/>
     </row>
-    <row r="22" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>3</v>
       </c>
@@ -6019,7 +6019,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -6031,7 +6031,7 @@
       </c>
       <c r="G23" s="16"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
@@ -6041,7 +6041,7 @@
       <c r="F24" s="14"/>
       <c r="G24" s="16"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -6051,7 +6051,7 @@
       <c r="F25" s="14"/>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -6061,7 +6061,7 @@
       <c r="F26" s="14"/>
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -6071,7 +6071,7 @@
       <c r="F27" s="14"/>
       <c r="G27" s="16"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -6081,7 +6081,7 @@
       <c r="F28" s="14"/>
       <c r="G28" s="16"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -6091,7 +6091,7 @@
       <c r="F29" s="14"/>
       <c r="G29" s="16"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
@@ -6101,7 +6101,7 @@
       <c r="F30" s="14"/>
       <c r="G30" s="16"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="51"/>
       <c r="B31" s="18"/>
       <c r="C31" s="19"/>
@@ -6135,7 +6135,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B33" s="45"/>
       <c r="C33" s="46"/>
       <c r="D33" s="46"/>
@@ -6147,7 +6147,7 @@
       </c>
       <c r="G33" s="47"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B34" s="45"/>
       <c r="C34" s="46"/>
       <c r="D34" s="46"/>
@@ -6157,7 +6157,7 @@
       <c r="F34" s="45"/>
       <c r="G34" s="47"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B35" s="45"/>
       <c r="C35" s="46"/>
       <c r="D35" s="46"/>
@@ -6167,7 +6167,7 @@
       <c r="F35" s="45"/>
       <c r="G35" s="47"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B36" s="45"/>
       <c r="C36" s="46"/>
       <c r="D36" s="46"/>
@@ -6177,7 +6177,7 @@
       <c r="F36" s="45"/>
       <c r="G36" s="47"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B37" s="45"/>
       <c r="C37" s="46"/>
       <c r="D37" s="46"/>
@@ -6187,7 +6187,7 @@
       <c r="F37" s="45"/>
       <c r="G37" s="47"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B38" s="45"/>
       <c r="C38" s="46"/>
       <c r="D38" s="46"/>
@@ -6197,7 +6197,7 @@
       <c r="F38" s="45"/>
       <c r="G38" s="47"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B39" s="45"/>
       <c r="C39" s="46"/>
       <c r="D39" s="46"/>
@@ -6207,7 +6207,7 @@
       <c r="F39" s="45"/>
       <c r="G39" s="47"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B40" s="45"/>
       <c r="C40" s="46"/>
       <c r="D40" s="46"/>
@@ -6217,7 +6217,7 @@
       <c r="F40" s="45"/>
       <c r="G40" s="47"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="51"/>
       <c r="B41" s="48"/>
       <c r="C41" s="49"/>
@@ -6230,7 +6230,7 @@
       </c>
       <c r="G41" s="50"/>
     </row>
-    <row r="42" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>5</v>
       </c>
@@ -6251,7 +6251,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B43" s="14"/>
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
@@ -6263,7 +6263,7 @@
       </c>
       <c r="G43" s="16"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B44" s="14"/>
       <c r="C44" s="15"/>
       <c r="D44" s="15"/>
@@ -6273,7 +6273,7 @@
       <c r="F44" s="14"/>
       <c r="G44" s="16"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B45" s="14"/>
       <c r="C45" s="15"/>
       <c r="D45" s="15"/>
@@ -6283,7 +6283,7 @@
       <c r="F45" s="14"/>
       <c r="G45" s="16"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B46" s="14"/>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
@@ -6293,7 +6293,7 @@
       <c r="F46" s="14"/>
       <c r="G46" s="16"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B47" s="14"/>
       <c r="C47" s="15"/>
       <c r="D47" s="15"/>
@@ -6303,7 +6303,7 @@
       <c r="F47" s="14"/>
       <c r="G47" s="16"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B48" s="14"/>
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
@@ -6313,7 +6313,7 @@
       <c r="F48" s="14"/>
       <c r="G48" s="16"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B49" s="14"/>
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
@@ -6323,7 +6323,7 @@
       <c r="F49" s="14"/>
       <c r="G49" s="16"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B50" s="14"/>
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
@@ -6333,7 +6333,7 @@
       <c r="F50" s="14"/>
       <c r="G50" s="16"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="51"/>
       <c r="B51" s="18"/>
       <c r="C51" s="19"/>
@@ -6367,7 +6367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="44"/>
       <c r="B53" s="45"/>
       <c r="C53" s="46"/>
@@ -6380,7 +6380,7 @@
       </c>
       <c r="G53" s="47"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="44"/>
       <c r="B54" s="45"/>
       <c r="C54" s="46"/>
@@ -6391,7 +6391,7 @@
       <c r="F54" s="45"/>
       <c r="G54" s="47"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="44"/>
       <c r="B55" s="45"/>
       <c r="C55" s="46"/>
@@ -6402,7 +6402,7 @@
       <c r="F55" s="45"/>
       <c r="G55" s="47"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="44"/>
       <c r="B56" s="45"/>
       <c r="C56" s="46"/>
@@ -6413,7 +6413,7 @@
       <c r="F56" s="45"/>
       <c r="G56" s="47"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="44"/>
       <c r="B57" s="45"/>
       <c r="C57" s="46"/>
@@ -6424,7 +6424,7 @@
       <c r="F57" s="45"/>
       <c r="G57" s="47"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="44"/>
       <c r="B58" s="45"/>
       <c r="C58" s="46"/>
@@ -6435,7 +6435,7 @@
       <c r="F58" s="45"/>
       <c r="G58" s="47"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="44"/>
       <c r="B59" s="45"/>
       <c r="C59" s="46"/>
@@ -6446,7 +6446,7 @@
       <c r="F59" s="45"/>
       <c r="G59" s="47"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="44"/>
       <c r="B60" s="45"/>
       <c r="C60" s="46"/>
@@ -6457,7 +6457,7 @@
       <c r="F60" s="45"/>
       <c r="G60" s="47"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="59"/>
       <c r="B61" s="48"/>
       <c r="C61" s="49"/>
@@ -6491,7 +6491,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="44"/>
       <c r="B63" s="45"/>
       <c r="C63" s="46"/>
@@ -6504,7 +6504,7 @@
       </c>
       <c r="G63" s="47"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="44"/>
       <c r="B64" s="45"/>
       <c r="C64" s="46"/>
@@ -6515,7 +6515,7 @@
       <c r="F64" s="45"/>
       <c r="G64" s="47"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="44"/>
       <c r="B65" s="45"/>
       <c r="C65" s="46"/>
@@ -6526,7 +6526,7 @@
       <c r="F65" s="45"/>
       <c r="G65" s="47"/>
     </row>
-    <row r="66" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="44"/>
       <c r="B66" s="45"/>
       <c r="C66" s="46"/>
@@ -6537,7 +6537,7 @@
       <c r="F66" s="45"/>
       <c r="G66" s="47"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="44"/>
       <c r="B67" s="45"/>
       <c r="C67" s="46"/>
@@ -6548,7 +6548,7 @@
       <c r="F67" s="45"/>
       <c r="G67" s="47"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="44"/>
       <c r="B68" s="45"/>
       <c r="C68" s="46"/>
@@ -6559,7 +6559,7 @@
       <c r="F68" s="45"/>
       <c r="G68" s="47"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="44"/>
       <c r="B69" s="45"/>
       <c r="C69" s="46"/>
@@ -6570,7 +6570,7 @@
       <c r="F69" s="45"/>
       <c r="G69" s="47"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="44"/>
       <c r="B70" s="45"/>
       <c r="C70" s="46"/>
@@ -6581,7 +6581,7 @@
       <c r="F70" s="45"/>
       <c r="G70" s="47"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="59"/>
       <c r="B71" s="48"/>
       <c r="C71" s="49"/>
@@ -6615,7 +6615,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="44"/>
       <c r="B73" s="45"/>
       <c r="C73" s="46"/>
@@ -6628,7 +6628,7 @@
       </c>
       <c r="G73" s="47"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="44"/>
       <c r="B74" s="45"/>
       <c r="C74" s="46"/>
@@ -6639,7 +6639,7 @@
       <c r="F74" s="45"/>
       <c r="G74" s="47"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="44"/>
       <c r="B75" s="45"/>
       <c r="C75" s="46"/>
@@ -6650,7 +6650,7 @@
       <c r="F75" s="45"/>
       <c r="G75" s="47"/>
     </row>
-    <row r="76" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="44"/>
       <c r="B76" s="45"/>
       <c r="C76" s="46"/>
@@ -6661,7 +6661,7 @@
       <c r="F76" s="45"/>
       <c r="G76" s="47"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="44"/>
       <c r="B77" s="45"/>
       <c r="C77" s="46"/>
@@ -6672,7 +6672,7 @@
       <c r="F77" s="45"/>
       <c r="G77" s="47"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="44"/>
       <c r="B78" s="45"/>
       <c r="C78" s="46"/>
@@ -6683,7 +6683,7 @@
       <c r="F78" s="45"/>
       <c r="G78" s="47"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="44"/>
       <c r="B79" s="45"/>
       <c r="C79" s="46"/>
@@ -6694,7 +6694,7 @@
       <c r="F79" s="45"/>
       <c r="G79" s="47"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="44"/>
       <c r="B80" s="45"/>
       <c r="C80" s="46"/>
@@ -6705,7 +6705,7 @@
       <c r="F80" s="45"/>
       <c r="G80" s="47"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="59"/>
       <c r="B81" s="48"/>
       <c r="C81" s="49"/>
@@ -6718,7 +6718,7 @@
       </c>
       <c r="G81" s="50"/>
     </row>
-    <row r="82" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="44">
         <v>9</v>
       </c>
@@ -6739,7 +6739,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="44"/>
       <c r="B83" s="45"/>
       <c r="C83" s="46"/>
@@ -6752,7 +6752,7 @@
       </c>
       <c r="G83" s="47"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="44"/>
       <c r="B84" s="45"/>
       <c r="C84" s="46"/>
@@ -6763,7 +6763,7 @@
       <c r="F84" s="45"/>
       <c r="G84" s="47"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="44"/>
       <c r="B85" s="45"/>
       <c r="C85" s="46"/>
@@ -6774,7 +6774,7 @@
       <c r="F85" s="45"/>
       <c r="G85" s="47"/>
     </row>
-    <row r="86" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="44"/>
       <c r="B86" s="45"/>
       <c r="C86" s="46"/>
@@ -6785,7 +6785,7 @@
       <c r="F86" s="45"/>
       <c r="G86" s="47"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="44"/>
       <c r="B87" s="45"/>
       <c r="C87" s="46"/>
@@ -6796,7 +6796,7 @@
       <c r="F87" s="45"/>
       <c r="G87" s="47"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="44"/>
       <c r="B88" s="45"/>
       <c r="C88" s="46"/>
@@ -6807,7 +6807,7 @@
       <c r="F88" s="45"/>
       <c r="G88" s="47"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="44"/>
       <c r="B89" s="45"/>
       <c r="C89" s="46"/>
@@ -6818,7 +6818,7 @@
       <c r="F89" s="45"/>
       <c r="G89" s="47"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="44"/>
       <c r="B90" s="45"/>
       <c r="C90" s="46"/>
@@ -6829,7 +6829,7 @@
       <c r="F90" s="45"/>
       <c r="G90" s="47"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="59"/>
       <c r="B91" s="48"/>
       <c r="C91" s="49"/>
@@ -6863,7 +6863,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="44"/>
       <c r="B93" s="45"/>
       <c r="C93" s="46"/>
@@ -6876,7 +6876,7 @@
       </c>
       <c r="G93" s="47"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="44"/>
       <c r="B94" s="45"/>
       <c r="C94" s="46"/>
@@ -6887,7 +6887,7 @@
       <c r="F94" s="45"/>
       <c r="G94" s="47"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="44"/>
       <c r="B95" s="45"/>
       <c r="C95" s="46"/>
@@ -6898,7 +6898,7 @@
       <c r="F95" s="45"/>
       <c r="G95" s="47"/>
     </row>
-    <row r="96" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="44"/>
       <c r="B96" s="45"/>
       <c r="C96" s="46"/>
@@ -6909,7 +6909,7 @@
       <c r="F96" s="45"/>
       <c r="G96" s="47"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="44"/>
       <c r="B97" s="45"/>
       <c r="C97" s="46"/>
@@ -6920,7 +6920,7 @@
       <c r="F97" s="45"/>
       <c r="G97" s="47"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="44"/>
       <c r="B98" s="45"/>
       <c r="C98" s="46"/>
@@ -6931,7 +6931,7 @@
       <c r="F98" s="45"/>
       <c r="G98" s="47"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="44"/>
       <c r="B99" s="45"/>
       <c r="C99" s="46"/>
@@ -6942,7 +6942,7 @@
       <c r="F99" s="45"/>
       <c r="G99" s="47"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="44"/>
       <c r="B100" s="45"/>
       <c r="C100" s="46"/>
@@ -6953,7 +6953,7 @@
       <c r="F100" s="45"/>
       <c r="G100" s="47"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="59"/>
       <c r="B101" s="48"/>
       <c r="C101" s="49"/>
@@ -6966,7 +6966,7 @@
       </c>
       <c r="G101" s="50"/>
     </row>
-    <row r="102" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="44">
         <v>11</v>
       </c>
@@ -6987,7 +6987,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="44"/>
       <c r="B103" s="45"/>
       <c r="C103" s="46"/>
@@ -7000,7 +7000,7 @@
       </c>
       <c r="G103" s="47"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" s="44"/>
       <c r="B104" s="45"/>
       <c r="C104" s="46"/>
@@ -7011,7 +7011,7 @@
       <c r="F104" s="45"/>
       <c r="G104" s="47"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="44"/>
       <c r="B105" s="45"/>
       <c r="C105" s="46"/>
@@ -7022,7 +7022,7 @@
       <c r="F105" s="45"/>
       <c r="G105" s="47"/>
     </row>
-    <row r="106" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="44"/>
       <c r="B106" s="45"/>
       <c r="C106" s="46"/>
@@ -7033,7 +7033,7 @@
       <c r="F106" s="45"/>
       <c r="G106" s="47"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="44"/>
       <c r="B107" s="45"/>
       <c r="C107" s="46"/>
@@ -7044,7 +7044,7 @@
       <c r="F107" s="45"/>
       <c r="G107" s="47"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="44"/>
       <c r="B108" s="45"/>
       <c r="C108" s="46"/>
@@ -7055,7 +7055,7 @@
       <c r="F108" s="45"/>
       <c r="G108" s="47"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="44"/>
       <c r="B109" s="45"/>
       <c r="C109" s="46"/>
@@ -7066,7 +7066,7 @@
       <c r="F109" s="45"/>
       <c r="G109" s="47"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="44"/>
       <c r="B110" s="45"/>
       <c r="C110" s="46"/>
@@ -7077,7 +7077,7 @@
       <c r="F110" s="45"/>
       <c r="G110" s="47"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="59"/>
       <c r="B111" s="48"/>
       <c r="C111" s="49"/>
@@ -7111,7 +7111,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="44"/>
       <c r="B113" s="45"/>
       <c r="C113" s="46"/>
@@ -7124,7 +7124,7 @@
       </c>
       <c r="G113" s="47"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="44"/>
       <c r="B114" s="45"/>
       <c r="C114" s="46"/>
@@ -7135,7 +7135,7 @@
       <c r="F114" s="45"/>
       <c r="G114" s="47"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="44"/>
       <c r="B115" s="45"/>
       <c r="C115" s="46"/>
@@ -7146,7 +7146,7 @@
       <c r="F115" s="45"/>
       <c r="G115" s="47"/>
     </row>
-    <row r="116" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="44"/>
       <c r="B116" s="45"/>
       <c r="C116" s="46"/>
@@ -7157,7 +7157,7 @@
       <c r="F116" s="45"/>
       <c r="G116" s="47"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="44"/>
       <c r="B117" s="45"/>
       <c r="C117" s="46"/>
@@ -7168,7 +7168,7 @@
       <c r="F117" s="45"/>
       <c r="G117" s="47"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="44"/>
       <c r="B118" s="45"/>
       <c r="C118" s="46"/>
@@ -7179,7 +7179,7 @@
       <c r="F118" s="45"/>
       <c r="G118" s="47"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="44"/>
       <c r="B119" s="45"/>
       <c r="C119" s="46"/>
@@ -7190,7 +7190,7 @@
       <c r="F119" s="45"/>
       <c r="G119" s="47"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="44"/>
       <c r="B120" s="45"/>
       <c r="C120" s="46"/>
@@ -7201,7 +7201,7 @@
       <c r="F120" s="45"/>
       <c r="G120" s="47"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="59"/>
       <c r="B121" s="48"/>
       <c r="C121" s="49"/>
@@ -7235,7 +7235,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="44"/>
       <c r="B123" s="45"/>
       <c r="C123" s="46"/>
@@ -7248,7 +7248,7 @@
       </c>
       <c r="G123" s="47"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="44"/>
       <c r="B124" s="45"/>
       <c r="C124" s="46"/>
@@ -7259,7 +7259,7 @@
       <c r="F124" s="45"/>
       <c r="G124" s="47"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="44"/>
       <c r="B125" s="45"/>
       <c r="C125" s="46"/>
@@ -7270,7 +7270,7 @@
       <c r="F125" s="45"/>
       <c r="G125" s="47"/>
     </row>
-    <row r="126" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="44"/>
       <c r="B126" s="45"/>
       <c r="C126" s="46"/>
@@ -7281,7 +7281,7 @@
       <c r="F126" s="45"/>
       <c r="G126" s="47"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="44"/>
       <c r="B127" s="45"/>
       <c r="C127" s="46"/>
@@ -7292,7 +7292,7 @@
       <c r="F127" s="45"/>
       <c r="G127" s="47"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" s="44"/>
       <c r="B128" s="45"/>
       <c r="C128" s="46"/>
@@ -7303,7 +7303,7 @@
       <c r="F128" s="45"/>
       <c r="G128" s="47"/>
     </row>
-    <row r="129" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" s="44"/>
       <c r="B129" s="45"/>
       <c r="C129" s="46"/>
@@ -7314,7 +7314,7 @@
       <c r="F129" s="45"/>
       <c r="G129" s="47"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" s="44"/>
       <c r="B130" s="45"/>
       <c r="C130" s="46"/>
@@ -7325,7 +7325,7 @@
       <c r="F130" s="45"/>
       <c r="G130" s="47"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="59"/>
       <c r="B131" s="48"/>
       <c r="C131" s="49"/>
@@ -7359,7 +7359,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" s="13"/>
       <c r="B133" s="14"/>
       <c r="C133" s="15"/>
@@ -7372,7 +7372,7 @@
       </c>
       <c r="G133" s="16"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="13"/>
       <c r="B134" s="14"/>
       <c r="C134" s="15"/>
@@ -7383,7 +7383,7 @@
       <c r="F134" s="14"/>
       <c r="G134" s="16"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="13"/>
       <c r="B135" s="14"/>
       <c r="C135" s="15"/>
@@ -7394,7 +7394,7 @@
       <c r="F135" s="14"/>
       <c r="G135" s="16"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="13"/>
       <c r="B136" s="14"/>
       <c r="C136" s="15"/>
@@ -7405,7 +7405,7 @@
       <c r="F136" s="14"/>
       <c r="G136" s="16"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="13"/>
       <c r="B137" s="14"/>
       <c r="C137" s="15"/>
@@ -7416,7 +7416,7 @@
       <c r="F137" s="14"/>
       <c r="G137" s="16"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" s="13"/>
       <c r="B138" s="14"/>
       <c r="C138" s="15"/>
@@ -7427,7 +7427,7 @@
       <c r="F138" s="14"/>
       <c r="G138" s="16"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="13"/>
       <c r="B139" s="14"/>
       <c r="C139" s="15"/>
@@ -7438,7 +7438,7 @@
       <c r="F139" s="14"/>
       <c r="G139" s="16"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" s="17"/>
       <c r="B140" s="18"/>
       <c r="C140" s="19"/>
@@ -7452,7 +7452,13 @@
       <c r="G140" s="20"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G140"/>
+  <autoFilter ref="A1:G140">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="High"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataConsolidate/>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
@@ -7467,8 +7473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7919,6 +7925,7 @@
       <c r="G31" s="20"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G31"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7927,8 +7934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8178,6 +8185,7 @@
       <c r="G16" s="20"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G16"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8186,9 +8194,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10001,7 +10009,7 @@
       <c r="G130" s="76"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G69"/>
+  <autoFilter ref="A1:G130"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10010,9 +10018,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10347,7 +10355,7 @@
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -10668,7 +10676,7 @@
       <c r="F46" s="85" t="s">
         <v>231</v>
       </c>
-      <c r="G46" s="95"/>
+      <c r="G46" s="94"/>
     </row>
     <row r="47" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="23">
@@ -10844,7 +10852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E16" sqref="E16:G16"/>
     </sheetView>
@@ -11051,10 +11059,10 @@
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51"/>
-      <c r="E13" s="99" t="s">
+      <c r="E13" s="98" t="s">
         <v>273</v>
       </c>
-      <c r="F13" s="100" t="s">
+      <c r="F13" s="99" t="s">
         <v>274</v>
       </c>
       <c r="G13" s="76"/>
@@ -11098,10 +11106,10 @@
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
       <c r="D16" s="51"/>
-      <c r="E16" s="99" t="s">
+      <c r="E16" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="F16" s="100" t="s">
+      <c r="F16" s="99" t="s">
         <v>254</v>
       </c>
       <c r="G16" s="76"/>
@@ -11116,7 +11124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
@@ -11323,10 +11331,10 @@
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51"/>
-      <c r="E13" s="99" t="s">
+      <c r="E13" s="98" t="s">
         <v>273</v>
       </c>
-      <c r="F13" s="100" t="s">
+      <c r="F13" s="99" t="s">
         <v>274</v>
       </c>
       <c r="G13" s="76"/>
@@ -11370,10 +11378,10 @@
       <c r="B16" s="51"/>
       <c r="C16" s="51"/>
       <c r="D16" s="51"/>
-      <c r="E16" s="99" t="s">
+      <c r="E16" s="98" t="s">
         <v>278</v>
       </c>
-      <c r="F16" s="100" t="s">
+      <c r="F16" s="99" t="s">
         <v>254</v>
       </c>
       <c r="G16" s="76"/>

</xml_diff>